<commit_message>
Worked through new cost variant files and more of LW155.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/JSF/Cleaned 09-F-1079_JSF_SARS_1996_Present.xlsx
+++ b/FOIA SAR data/JSF/Cleaned 09-F-1079_JSF_SARS_1996_Present.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2015-09 Joint Development\Research\JSF F-35\Current Change explanations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2007-01 PROFESSIONAL SERVICES\R scripts and data\FOIA SAR data\JSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25155" windowHeight="6105"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -489,26 +489,26 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -865,10 +865,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -984,10 +984,10 @@
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="21"/>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -1001,112 +1001,112 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="16">
         <v>-81.599999999999994</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="16" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="16">
         <v>-14.5</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="16">
         <v>-16.600000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="16">
         <v>-2341.1999999999998</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="16">
         <v>-3576.3</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="16">
         <v>-3414.7</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="16">
         <v>-5201.3999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="16" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="16" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1114,10 +1114,10 @@
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="16"/>
+      <c r="C24" s="21"/>
     </row>
     <row r="25" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">

</xml_diff>